<commit_message>
Motor Caracterization Symbols and Names
</commit_message>
<xml_diff>
--- a/Motor Characterization.xlsx
+++ b/Motor Characterization.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c13bde81646cda71/Escritorio/Enerdrais/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="8_{F0BFD4FD-6D25-4A3D-8EF6-A4C21AAF60BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED9DC2F1-FE3A-4BEF-A3BF-3EF33A5890BC}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="8_{F0BFD4FD-6D25-4A3D-8EF6-A4C21AAF60BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BEEABD2-9997-456A-B083-4B759DEF5E7D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89945170-611C-4268-B67E-7A04A5D26ECF}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{89945170-611C-4268-B67E-7A04A5D26ECF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="61">
   <si>
     <t>Column1</t>
   </si>
@@ -51,15 +52,190 @@
   </si>
   <si>
     <t xml:space="preserve">Motor 1: </t>
+  </si>
+  <si>
+    <t>Constante de Tiempo Térmica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impedancia Térmica </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Temperatura máxima </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constante de tiempo mecánica </t>
+  </si>
+  <si>
+    <t>Constante de Tiempo eléctrica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inercia del Rotor </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fricción de Torque </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constante del Motor </t>
+  </si>
+  <si>
+    <t>Corriente pico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corriente sin Carga </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inductancia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Resistencia </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constante Back </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torque Constante </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peso </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torque Pico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Torque Continuo Máximo </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocidad Sin Carga </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltaje de Referencia </t>
+  </si>
+  <si>
+    <t>Parametro</t>
+  </si>
+  <si>
+    <t>Simbolo</t>
+  </si>
+  <si>
+    <t>Unidades</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>SNl</t>
+  </si>
+  <si>
+    <t>Tc</t>
+  </si>
+  <si>
+    <t>Tpk</t>
+  </si>
+  <si>
+    <t>Wm</t>
+  </si>
+  <si>
+    <t>Kt</t>
+  </si>
+  <si>
+    <t>Ke</t>
+  </si>
+  <si>
+    <t>Rt</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>Inl</t>
+  </si>
+  <si>
+    <t>Ip</t>
+  </si>
+  <si>
+    <t>Km</t>
+  </si>
+  <si>
+    <t>Tf</t>
+  </si>
+  <si>
+    <t>Jm</t>
+  </si>
+  <si>
+    <t>te</t>
+  </si>
+  <si>
+    <t>tm</t>
+  </si>
+  <si>
+    <t>Tmax</t>
+  </si>
+  <si>
+    <t>Rth</t>
+  </si>
+  <si>
+    <t>tT</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>rpm</t>
+  </si>
+  <si>
+    <t>Nm</t>
+  </si>
+  <si>
+    <t>oz</t>
+  </si>
+  <si>
+    <t>N-m/A</t>
+  </si>
+  <si>
+    <t>V/Krpm</t>
+  </si>
+  <si>
+    <t>Ohms</t>
+  </si>
+  <si>
+    <t>mH</t>
+  </si>
+  <si>
+    <t>Nm/W</t>
+  </si>
+  <si>
+    <t>Kgm2</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>ºC</t>
+  </si>
+  <si>
+    <t>ºC/watt</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -74,7 +250,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -82,20 +258,843 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="34">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -106,7 +1105,7 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="1" xr9:uid="{E0BB3733-6632-4A27-8A4D-4DF45042573A}">
-      <tableStyleElement type="wholeTable" dxfId="0"/>
+      <tableStyleElement type="wholeTable" dxfId="33"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -120,53 +1119,57 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63E027B4-77EB-4572-A7E3-4C2695C30681}" name="Table1" displayName="Table1" ref="A2:D22" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63E027B4-77EB-4572-A7E3-4C2695C30681}" name="Table1" displayName="Table1" ref="A2:D22" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
   <autoFilter ref="A2:D22" xr:uid="{63E027B4-77EB-4572-A7E3-4C2695C30681}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8B524A04-117F-4933-B428-AFB5C6095C86}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{6665E97C-1AF8-4C09-A274-46B7055634CB}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{D6669256-5714-47D7-9147-6A00FBCCFF52}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{CB519FBA-C8FF-4A17-BD64-11B439AA496F}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{8B524A04-117F-4933-B428-AFB5C6095C86}" name="Parametro" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{6665E97C-1AF8-4C09-A274-46B7055634CB}" name="Simbolo" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{D6669256-5714-47D7-9147-6A00FBCCFF52}" name="Unidades" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{CB519FBA-C8FF-4A17-BD64-11B439AA496F}" name="Column4" dataDxfId="29"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2740EAC2-40F7-49E8-AAED-A343E5D02E86}" name="Table13" displayName="Table13" ref="F2:I22" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{2740EAC2-40F7-49E8-AAED-A343E5D02E86}" name="Table13" displayName="Table13" ref="F2:I22" totalsRowShown="0" headerRowDxfId="16" dataDxfId="26" headerRowBorderDxfId="22" tableBorderDxfId="23" totalsRowBorderDxfId="21">
   <autoFilter ref="F2:I22" xr:uid="{2740EAC2-40F7-49E8-AAED-A343E5D02E86}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{DD5B539D-934F-4F24-B96D-7F37D0EBC5A7}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{D53818C0-56E3-4336-A83D-4AB8F1DAE836}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{D25B0AAB-BE76-4EC2-AC36-26C358971B3D}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{F22E7FA6-3A33-4CD7-A054-F914A186ED38}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{DD5B539D-934F-4F24-B96D-7F37D0EBC5A7}" name="Column1" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{D53818C0-56E3-4336-A83D-4AB8F1DAE836}" name="Column2" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{D25B0AAB-BE76-4EC2-AC36-26C358971B3D}" name="Column3" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{F22E7FA6-3A33-4CD7-A054-F914A186ED38}" name="Column4" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F54E1C1-4A9F-48AC-A116-3602D9200934}" name="Table14" displayName="Table14" ref="K2:N22" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F54E1C1-4A9F-48AC-A116-3602D9200934}" name="Table14" displayName="Table14" ref="K2:N22" totalsRowShown="0" headerRowDxfId="8" dataDxfId="25" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
   <autoFilter ref="K2:N22" xr:uid="{8F54E1C1-4A9F-48AC-A116-3602D9200934}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{299C9324-F7CF-4433-ABF0-750BF2FA28F9}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{7FF9FF65-ED06-4B73-89D2-EA84560251E3}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{5025E02A-12EB-4AF9-8330-DFD4080D4523}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{F7C76DE5-E246-4143-B415-A225711CCF41}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{299C9324-F7CF-4433-ABF0-750BF2FA28F9}" name="Column1" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7FF9FF65-ED06-4B73-89D2-EA84560251E3}" name="Column2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{5025E02A-12EB-4AF9-8330-DFD4080D4523}" name="Column3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{F7C76DE5-E246-4143-B415-A225711CCF41}" name="Column4" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0D2826BD-1206-4085-969A-D79FDCBBF09C}" name="Table15" displayName="Table15" ref="P2:S22" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0D2826BD-1206-4085-969A-D79FDCBBF09C}" name="Table15" displayName="Table15" ref="P2:S22" totalsRowShown="0" headerRowDxfId="0" dataDxfId="24" headerRowBorderDxfId="6" tableBorderDxfId="7" totalsRowBorderDxfId="5">
   <autoFilter ref="P2:S22" xr:uid="{0D2826BD-1206-4085-969A-D79FDCBBF09C}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{90DF3E47-D15A-4320-8CFF-F5F4C522E8C2}" name="Column1"/>
-    <tableColumn id="2" xr3:uid="{AA7F8EE1-C2E1-4C6A-B422-2D830F0CF52E}" name="Column2"/>
-    <tableColumn id="3" xr3:uid="{B1542A31-EA12-4CEB-BFE1-01462CF63338}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{F5A38761-01BB-425A-ABDA-6420A076C1BF}" name="Column4"/>
+    <tableColumn id="1" xr3:uid="{90DF3E47-D15A-4320-8CFF-F5F4C522E8C2}" name="Column1" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{AA7F8EE1-C2E1-4C6A-B422-2D830F0CF52E}" name="Column2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{B1542A31-EA12-4CEB-BFE1-01462CF63338}" name="Column3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{F5A38761-01BB-425A-ABDA-6420A076C1BF}" name="Column4" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -489,15 +1492,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A833C82-934B-4C70-A298-1D74AE5934AB}">
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11" customWidth="1"/>
+    <col min="1" max="1" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -526,55 +1531,592 @@
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="2"/>
+      <c r="F2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="J2" s="2"/>
+      <c r="K2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="G2" t="s">
+      <c r="L2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="H2" t="s">
+      <c r="M2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="N2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K2" t="s">
+      <c r="O2" s="2"/>
+      <c r="P2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="L2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="M2" t="s">
+      <c r="R2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="N2" t="s">
+      <c r="S2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="P2" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R2" t="s">
-        <v>2</v>
-      </c>
-      <c r="S2" t="s">
-        <v>3</v>
-      </c>
+    </row>
+    <row r="3" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="8"/>
+    </row>
+    <row r="4" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="7"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="2"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="8"/>
+    </row>
+    <row r="6" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="8"/>
+    </row>
+    <row r="7" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="7"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="8"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="8"/>
+    </row>
+    <row r="8" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="7"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="8"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="8"/>
+    </row>
+    <row r="9" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="7"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="2"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="8"/>
+    </row>
+    <row r="10" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="7"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="8"/>
+    </row>
+    <row r="11" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="7"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="2"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="8"/>
+    </row>
+    <row r="12" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="7"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="8"/>
+    </row>
+    <row r="13" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="2"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="2"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="8"/>
+      <c r="O17" s="2"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="8"/>
+    </row>
+    <row r="18" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="8"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+      <c r="S18" s="8"/>
+    </row>
+    <row r="19" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="7"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="3"/>
+      <c r="S20" s="8"/>
+    </row>
+    <row r="21" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="7"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="3"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="10"/>
+      <c r="H22" s="10"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="10"/>
+      <c r="M22" s="10"/>
+      <c r="N22" s="11"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="10"/>
+      <c r="R22" s="10"/>
+      <c r="S22" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -592,4 +2134,117 @@
     <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB927944-6959-48CC-B03A-EA3DD9BF4888}">
+  <dimension ref="A1:A19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A19" sqref="A1:A19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="52.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
MechaBible Mark I: Enedrais - Motor Caracterization thesis pdf
</commit_message>
<xml_diff>
--- a/Motor Characterization.xlsx
+++ b/Motor Characterization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\OneDrive\Documents\The_MechaBible\r_BeVisioneers_Enerdrais_ENG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390622A0-7460-4600-B1E3-4DDDCD100607}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{835F85BF-B6FF-41B0-8E6D-269541E55EFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{89945170-611C-4268-B67E-7A04A5D26ECF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="65">
   <si>
     <t xml:space="preserve">Motor 1: </t>
   </si>
@@ -177,12 +177,6 @@
     <t>Nm</t>
   </si>
   <si>
-    <t>oz</t>
-  </si>
-  <si>
-    <t>N-m/A</t>
-  </si>
-  <si>
     <t>V/Krpm</t>
   </si>
   <si>
@@ -216,20 +210,35 @@
     <t xml:space="preserve">Motor 2: </t>
   </si>
   <si>
-    <t xml:space="preserve">Motor 3: </t>
-  </si>
-  <si>
     <t xml:space="preserve">Motor 4: </t>
   </si>
   <si>
     <t>Constante Back - EMF</t>
+  </si>
+  <si>
+    <t>Motor 3: Odrive D6374-150KV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Constante de velocidad </t>
+  </si>
+  <si>
+    <t>Kv</t>
+  </si>
+  <si>
+    <t>rpm/V</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>Nm/A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,16 +269,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -305,22 +335,111 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1050,6 +1169,218 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>737287</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>67860</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1087221" cy="461024"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{674A27FD-1F42-B9BB-7A42-FFB3F4CD13EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12306808" y="5584311"/>
+              <a:ext cx="1087221" cy="461024"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:r>
+                      <a:rPr lang="es-MX" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝐽𝑚</m:t>
+                    </m:r>
+                    <m:r>
+                      <a:rPr lang="es-MX" sz="1600" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>=</m:t>
+                    </m:r>
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-MX" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <a:rPr lang="es-MX" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="es-MX" sz="1600" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                    <m:r>
+                      <a:rPr lang="es-MX" sz="1600" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>𝑚</m:t>
+                    </m:r>
+                    <m:sSup>
+                      <m:sSupPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="es-MX" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSupPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="es-MX" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑟</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sup>
+                        <m:r>
+                          <a:rPr lang="es-MX" sz="1600" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:sup>
+                    </m:sSup>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="es-MX" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="CuadroTexto 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{674A27FD-1F42-B9BB-7A42-FFB3F4CD13EE}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="12306808" y="5584311"/>
+              <a:ext cx="1087221" cy="461024"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="es-MX" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝐽𝑚</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-MX" sz="1600" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>=</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-MX" sz="1600" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>1/2 𝑚</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="es-MX" sz="1600" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑟^2</a:t>
+              </a:r>
+              <a:endParaRPr lang="es-MX" sz="1600"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1423,8 +1754,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A833C82-934B-4C70-A298-1D74AE5934AB}">
   <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1446,31 +1777,31 @@
     <col min="19" max="19" width="14.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="9"/>
       <c r="F1" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
+        <v>56</v>
+      </c>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
       <c r="K1" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="9"/>
       <c r="P1" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
+        <v>57</v>
+      </c>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="9"/>
     </row>
     <row r="2" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1483,7 +1814,7 @@
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="2" t="s">
@@ -1496,7 +1827,7 @@
         <v>22</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="J2" s="1"/>
       <c r="K2" s="2" t="s">
@@ -1509,7 +1840,7 @@
         <v>22</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="O2" s="1"/>
       <c r="P2" s="2" t="s">
@@ -1522,7 +1853,7 @@
         <v>22</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.35">
@@ -1557,7 +1888,9 @@
       <c r="M3" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="N3" s="2"/>
+      <c r="N3" s="2">
+        <v>48</v>
+      </c>
       <c r="O3" s="1"/>
       <c r="P3" s="2" t="s">
         <v>19</v>
@@ -1602,7 +1935,9 @@
       <c r="M4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2">
+        <v>5760</v>
+      </c>
       <c r="O4" s="1"/>
       <c r="P4" s="2" t="s">
         <v>18</v>
@@ -1647,7 +1982,9 @@
       <c r="M5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>3.86</v>
+      </c>
       <c r="O5" s="1"/>
       <c r="P5" s="2" t="s">
         <v>17</v>
@@ -1713,7 +2050,7 @@
         <v>28</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="1"/>
@@ -1724,7 +2061,7 @@
         <v>28</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="1"/>
@@ -1735,9 +2072,11 @@
         <v>28</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="N7" s="2"/>
+        <v>63</v>
+      </c>
+      <c r="N7" s="2">
+        <v>0.89</v>
+      </c>
       <c r="O7" s="1"/>
       <c r="P7" s="2" t="s">
         <v>15</v>
@@ -1746,7 +2085,7 @@
         <v>28</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="S7" s="2"/>
     </row>
@@ -1758,7 +2097,7 @@
         <v>29</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="1"/>
@@ -1769,7 +2108,7 @@
         <v>29</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="I8" s="2"/>
       <c r="J8" s="1"/>
@@ -1780,7 +2119,7 @@
         <v>29</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="1"/>
@@ -1791,196 +2130,202 @@
         <v>29</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="S8" s="2"/>
     </row>
     <row r="9" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="1"/>
       <c r="K9" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="N9" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="N9" s="2">
+        <v>6.6600000000000001E-3</v>
+      </c>
       <c r="O9" s="1"/>
       <c r="P9" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>30</v>
       </c>
       <c r="R9" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="S9" s="2"/>
     </row>
     <row r="10" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="D10" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="I10" s="6"/>
       <c r="J10" s="1"/>
       <c r="K10" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="N10" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="N10" s="2">
+        <v>150</v>
+      </c>
       <c r="O10" s="1"/>
       <c r="P10" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="S10" s="6"/>
     </row>
     <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D11" s="2"/>
       <c r="E11" s="1"/>
       <c r="F11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="1"/>
       <c r="K11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="N11" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="N11" s="2">
+        <v>3.9E-2</v>
+      </c>
       <c r="O11" s="1"/>
       <c r="P11" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="S11" s="2"/>
     </row>
     <row r="12" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
       <c r="F12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="I12" s="2"/>
-      <c r="J12" s="6"/>
+      <c r="J12" s="5"/>
       <c r="K12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" s="1"/>
       <c r="P12" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="R12" s="2" t="s">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="S12" s="2"/>
     </row>
     <row r="13" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>24</v>
@@ -1988,10 +2333,10 @@
       <c r="D13" s="2"/>
       <c r="E13" s="1"/>
       <c r="F13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>24</v>
@@ -1999,21 +2344,21 @@
       <c r="I13" s="2"/>
       <c r="J13" s="1"/>
       <c r="K13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="N13" s="2"/>
+      <c r="N13" s="10"/>
       <c r="O13" s="1"/>
       <c r="P13" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R13" s="2" t="s">
         <v>24</v>
@@ -2022,394 +2367,441 @@
     </row>
     <row r="14" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="1"/>
       <c r="F14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="1"/>
       <c r="K14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="N14" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="N14" s="2">
+        <v>70</v>
+      </c>
       <c r="O14" s="1"/>
       <c r="P14" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="R14" s="2" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="S14" s="2"/>
     </row>
     <row r="15" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="1"/>
       <c r="F15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="1"/>
       <c r="K15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M15" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="N15" s="2"/>
+        <v>49</v>
+      </c>
+      <c r="N15" s="2">
+        <v>0.23</v>
+      </c>
       <c r="O15" s="1"/>
       <c r="P15" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="S15" s="2"/>
     </row>
     <row r="16" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="1"/>
       <c r="F16" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="1"/>
       <c r="K16" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="N16" s="2"/>
       <c r="O16" s="1"/>
       <c r="P16" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="R16" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="S16" s="2"/>
     </row>
     <row r="17" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="1"/>
       <c r="F17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="1"/>
       <c r="K17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="N17" s="2"/>
       <c r="O17" s="1"/>
       <c r="P17" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="S17" s="2"/>
     </row>
     <row r="18" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="1"/>
       <c r="F18" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="1"/>
       <c r="K18" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="N18" s="2"/>
       <c r="O18" s="1"/>
       <c r="P18" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="S18" s="2"/>
     </row>
     <row r="19" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="1"/>
       <c r="F19" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="1"/>
       <c r="K19" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="1"/>
       <c r="P19" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="S19" s="2"/>
     </row>
     <row r="20" spans="1:19" ht="18" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="1"/>
       <c r="F20" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="1"/>
       <c r="K20" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N20" s="2"/>
       <c r="O20" s="1"/>
       <c r="P20" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="Q20" s="2" t="s">
+      <c r="B21" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="R20" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="S20" s="2"/>
-    </row>
-    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="C21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" s="2"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N21" s="2"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="3" t="s">
+      <c r="C22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="F22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="H21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I21" s="3"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="3" t="s">
+      <c r="H22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="3"/>
+      <c r="K22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="L22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="M21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="N21" s="3"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="3" t="s">
+      <c r="M22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="N22" s="3"/>
+      <c r="P22" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="Q21" s="3" t="s">
+      <c r="Q22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R21" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="S21" s="3"/>
-    </row>
-    <row r="22" spans="1:19" ht="18" x14ac:dyDescent="0.35">
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I23" s="8"/>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="I25" s="5"/>
+      <c r="R22" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="S22" s="3"/>
+    </row>
+    <row r="25" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K28" s="13"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="F29" s="5"/>
+      <c r="F29" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="F1:I1"/>
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="P1:S1"/>
+    <mergeCell ref="K26:K28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="4">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
MechaBible Mark I: Enedrais - Motor Caracterization translation
</commit_message>
<xml_diff>
--- a/Motor Characterization.xlsx
+++ b/Motor Characterization.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\OneDrive\Documents\The_MechaBible\r_BeVisioneers_Enerdrais_ENG\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013CA439-8E2F-4B60-8584-4F9722C73C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB6A2719-08CB-4F36-BB53-ECD41299C877}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{89945170-611C-4268-B67E-7A04A5D26ECF}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="65">
   <si>
     <t>Constante de Tiempo Térmica</t>
   </si>
@@ -96,15 +96,6 @@
     <t xml:space="preserve">Voltaje de Referencia </t>
   </si>
   <si>
-    <t>Parametro</t>
-  </si>
-  <si>
-    <t>Simbolo</t>
-  </si>
-  <si>
-    <t>Unidades</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
@@ -171,18 +162,6 @@
     <t>ms</t>
   </si>
   <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Constante Back - EMF</t>
-  </si>
-  <si>
-    <t>Motor 3: Odrive D6374-150KV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Constante de velocidad </t>
-  </si>
-  <si>
     <t>Kv</t>
   </si>
   <si>
@@ -196,6 +175,63 @@
   </si>
   <si>
     <t>Motor 1: Odrive D5312-330KV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maximum continuous torque </t>
+  </si>
+  <si>
+    <t>Weight</t>
+  </si>
+  <si>
+    <t>Constant torque</t>
+  </si>
+  <si>
+    <t>Back Constant - EMF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Velocity constant </t>
+  </si>
+  <si>
+    <t>Resistence</t>
+  </si>
+  <si>
+    <t>Spike current</t>
+  </si>
+  <si>
+    <t>Motor constant</t>
+  </si>
+  <si>
+    <t>Rotor inertia</t>
+  </si>
+  <si>
+    <t>Electric time constant</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Simbol</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Spike torque</t>
+  </si>
+  <si>
+    <t>No load velocity</t>
+  </si>
+  <si>
+    <t>Reference voltage</t>
+  </si>
+  <si>
+    <t>Mechanical time constant</t>
+  </si>
+  <si>
+    <t>Motor 2: Odrive D6374-150KV</t>
   </si>
 </sst>
 </file>
@@ -228,7 +264,7 @@
     <font>
       <b/>
       <sz val="14"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -404,7 +440,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -412,6 +448,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,7 +462,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
@@ -439,6 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -448,13 +487,187 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -488,182 +701,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -789,8 +826,8 @@
       <xdr:rowOff>121521</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1087221" cy="345672"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -915,7 +952,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="CuadroTexto 1">
@@ -998,8 +1035,8 @@
       <xdr:rowOff>14947</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1087221" cy="189604"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -1074,7 +1111,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="CuadroTexto 2">
@@ -1151,8 +1188,8 @@
       <xdr:rowOff>91470</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1267522" cy="346954"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3">
@@ -1267,7 +1304,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="4" name="CuadroTexto 3">
@@ -1356,8 +1393,8 @@
       <xdr:rowOff>104349</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1267522" cy="346890"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CuadroTexto 4">
@@ -1475,7 +1512,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="CuadroTexto 4">
@@ -1552,8 +1589,8 @@
       <xdr:rowOff>4217</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1407045" cy="189604"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CuadroTexto 5">
@@ -1634,7 +1671,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="6" name="CuadroTexto 5">
@@ -1710,23 +1747,23 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{63E027B4-77EB-4572-A7E3-4C2695C30681}" name="Table1" displayName="Table1" ref="B3:E16" totalsRowShown="0" headerRowDxfId="14" dataDxfId="13">
   <autoFilter ref="B3:E16" xr:uid="{63E027B4-77EB-4572-A7E3-4C2695C30681}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8B524A04-117F-4933-B428-AFB5C6095C86}" name="Parametro" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{6665E97C-1AF8-4C09-A274-46B7055634CB}" name="Simbolo" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{D6669256-5714-47D7-9147-6A00FBCCFF52}" name="Unidades" dataDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{CB519FBA-C8FF-4A17-BD64-11B439AA496F}" name="Valor" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{8B524A04-117F-4933-B428-AFB5C6095C86}" name="Parameter" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{6665E97C-1AF8-4C09-A274-46B7055634CB}" name="Simbol" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{D6669256-5714-47D7-9147-6A00FBCCFF52}" name="Unit" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{CB519FBA-C8FF-4A17-BD64-11B439AA496F}" name="Value" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F54E1C1-4A9F-48AC-A116-3602D9200934}" name="Table14" displayName="Table14" ref="G3:J16" totalsRowShown="0" headerRowDxfId="0" dataDxfId="8" headerRowBorderDxfId="1" tableBorderDxfId="7" totalsRowBorderDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8F54E1C1-4A9F-48AC-A116-3602D9200934}" name="Table14" displayName="Table14" ref="G3:J16" totalsRowShown="0" headerRowDxfId="8" dataDxfId="6" headerRowBorderDxfId="7" tableBorderDxfId="5" totalsRowBorderDxfId="4">
   <autoFilter ref="G3:J16" xr:uid="{8F54E1C1-4A9F-48AC-A116-3602D9200934}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{299C9324-F7CF-4433-ABF0-750BF2FA28F9}" name="Parametro" dataDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{7FF9FF65-ED06-4B73-89D2-EA84560251E3}" name="Simbolo" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{5025E02A-12EB-4AF9-8330-DFD4080D4523}" name="Unidades" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{F7C76DE5-E246-4143-B415-A225711CCF41}" name="Valor" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{299C9324-F7CF-4433-ABF0-750BF2FA28F9}" name="Parameter" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{7FF9FF65-ED06-4B73-89D2-EA84560251E3}" name="Simbol" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{5025E02A-12EB-4AF9-8330-DFD4080D4523}" name="Unit" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{F7C76DE5-E246-4143-B415-A225711CCF41}" name="Value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2052,7 +2089,7 @@
   <dimension ref="A2:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16:J16"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2077,420 +2114,421 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="16"/>
-      <c r="G2" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="16"/>
+      <c r="B2" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="19"/>
+      <c r="G2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="19"/>
     </row>
     <row r="3" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="17" t="s">
+      <c r="D4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" s="17" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="4" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="J4" s="18">
+      <c r="I4" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="6">
         <v>48</v>
       </c>
     </row>
     <row r="5" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="J5" s="2">
         <v>5760</v>
       </c>
     </row>
     <row r="6" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E6" s="18">
+      <c r="B6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="6">
         <v>0.75</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="H6" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="I6" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="J6" s="18">
+      <c r="G6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J6" s="6">
         <v>3.86</v>
       </c>
     </row>
     <row r="7" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" s="2">
         <v>1.5</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="J7" s="2">
         <v>7.72</v>
       </c>
     </row>
     <row r="8" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" s="18"/>
+      <c r="B8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="6"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="18">
+      <c r="G8" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="J8" s="6">
         <v>0.89</v>
       </c>
     </row>
     <row r="9" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E9" s="2">
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="J9" s="2">
         <v>6.3700000000000007E-2</v>
       </c>
     </row>
     <row r="10" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B10" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="E10" s="18">
+      <c r="B10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="6">
         <v>3.0000000000000001E-3</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="18" t="s">
-        <v>29</v>
-      </c>
-      <c r="I10" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="J10" s="18">
+      <c r="G10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="J10" s="6">
         <v>3.8E-3</v>
       </c>
     </row>
     <row r="11" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E11" s="2">
         <v>330</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="J11" s="2">
         <v>150</v>
       </c>
     </row>
     <row r="12" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B12" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" s="18">
+      <c r="B12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="6">
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="F12" s="1"/>
-      <c r="G12" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="18" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="J12" s="18">
+      <c r="G12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J12" s="6">
         <v>3.9E-2</v>
       </c>
     </row>
     <row r="13" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E13" s="2">
         <v>60</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="2" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="J13" s="2">
         <v>70</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B14" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="18"/>
+      <c r="B14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="6"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="H14" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="J14" s="18">
+      <c r="G14" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" s="6">
         <v>0.23</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="18" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="1"/>
       <c r="G15" s="2" t="s">
-        <v>5</v>
+        <v>54</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="J15" s="2">
         <v>4.5000000000000003E-5</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="B16" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="E16" s="18"/>
+      <c r="B16" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="6"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="18" t="s">
-        <v>3</v>
-      </c>
-      <c r="H16" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="J16" s="18">
+      <c r="G16" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="6">
         <v>21.75</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="F17" s="1"/>
+      <c r="G17" s="16"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="5"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="9"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B19" s="8"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="9"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="10"/>
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="12"/>
-      <c r="J20" s="13"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="15"/>
     </row>
     <row r="21" spans="1:15" ht="18" x14ac:dyDescent="0.35">
       <c r="E21" s="1"/>

</xml_diff>